<commit_message>
feat: add sdel pek luch
</commit_message>
<xml_diff>
--- a/app/detailed_sales_report.xlsx
+++ b/app/detailed_sales_report.xlsx
@@ -519,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -672,27 +672,27 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>10.12.2024</t>
+          <t>21.02.2025</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Прямая</t>
+          <t>ПЭК</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>2 продуктов</t>
+          <t>1 продуктов</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>1 осн.</t>
+          <t>0 осн.</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr"/>
@@ -715,7 +715,7 @@
       <c r="P2" s="3" t="n"/>
       <c r="Q2" s="3" t="n"/>
       <c r="R2" s="3" t="n">
-        <v>900</v>
+        <v>200</v>
       </c>
       <c r="S2" s="3" t="n">
         <v>0</v>
@@ -724,42 +724,42 @@
         <v>0</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>120</v>
+        <v>2000</v>
       </c>
       <c r="V2" s="3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="W2" s="3" t="n">
-        <v>120</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" s="5" t="n">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>10.12.2024</t>
+          <t>21.02.2025</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Прямая</t>
+          <t>ПЭК</t>
         </is>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>Таежная</t>
+          <t>Корзинка белая</t>
         </is>
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>1990 - 5 частей</t>
         </is>
       </c>
       <c r="F3" s="6" t="inlineStr">
         <is>
-          <t>Да</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="G3" s="6" t="inlineStr">
@@ -792,217 +792,211 @@
       <c r="V3" s="6" t="inlineStr"/>
       <c r="W3" s="6" t="inlineStr"/>
     </row>
-    <row r="4" outlineLevel="1">
-      <c r="A4" s="5" t="n">
-        <v>899</v>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>10.12.2024</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>Прямая</t>
-        </is>
-      </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>Гирлянда мишура</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>30м</t>
-        </is>
-      </c>
-      <c r="F4" s="6" t="inlineStr">
-        <is>
-          <t>Нет</t>
-        </is>
-      </c>
-      <c r="G4" s="6" t="inlineStr">
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>901</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>21.02.2025</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>СДЭК</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>1 продуктов</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr"/>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>1 осн.</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr"/>
+      <c r="H4" s="3" t="inlineStr"/>
+      <c r="I4" s="3" t="inlineStr"/>
+      <c r="J4" s="3" t="inlineStr"/>
+      <c r="K4" s="4" t="inlineStr">
         <is>
           <t>Закрыт</t>
         </is>
       </c>
-      <c r="H4" s="6" t="n"/>
-      <c r="I4" s="6" t="inlineStr"/>
-      <c r="J4" s="6" t="inlineStr"/>
-      <c r="K4" s="7" t="inlineStr">
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>Леша разраб (@Ni3omi)</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr"/>
+      <c r="N4" s="3" t="inlineStr"/>
+      <c r="O4" s="3" t="inlineStr"/>
+      <c r="P4" s="3" t="n"/>
+      <c r="Q4" s="3" t="n"/>
+      <c r="R4" s="3" t="n">
+        <v>800</v>
+      </c>
+      <c r="S4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>200</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="5" outlineLevel="1">
+      <c r="A5" s="5" t="n">
+        <v>901</v>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>21.02.2025</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>СДЭК</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Королевская литая</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Закрыт</t>
         </is>
       </c>
-      <c r="L4" s="7" t="inlineStr">
+      <c r="H5" s="6" t="n"/>
+      <c r="I5" s="6" t="inlineStr"/>
+      <c r="J5" s="6" t="inlineStr"/>
+      <c r="K5" s="7" t="inlineStr">
+        <is>
+          <t>Закрыт</t>
+        </is>
+      </c>
+      <c r="L5" s="7" t="inlineStr">
         <is>
           <t>Леша разраб (@Ni3omi)</t>
         </is>
       </c>
-      <c r="M4" s="6" t="inlineStr"/>
-      <c r="N4" s="6" t="inlineStr"/>
-      <c r="O4" s="6" t="inlineStr"/>
-      <c r="P4" s="6" t="inlineStr"/>
-      <c r="Q4" s="6" t="inlineStr"/>
-      <c r="R4" s="6" t="inlineStr"/>
-      <c r="S4" s="6" t="inlineStr"/>
-      <c r="T4" s="6" t="inlineStr"/>
-      <c r="U4" s="6" t="inlineStr"/>
-      <c r="V4" s="6" t="inlineStr"/>
-      <c r="W4" s="6" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>898</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>09.12.2024</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Прямая</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>2 продуктов</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr"/>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>1 осн.</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr"/>
-      <c r="H5" s="3" t="inlineStr"/>
-      <c r="I5" s="3" t="inlineStr"/>
-      <c r="J5" s="3" t="inlineStr"/>
-      <c r="K5" s="4" t="inlineStr">
+      <c r="M5" s="6" t="inlineStr"/>
+      <c r="N5" s="6" t="inlineStr"/>
+      <c r="O5" s="6" t="inlineStr"/>
+      <c r="P5" s="6" t="inlineStr"/>
+      <c r="Q5" s="6" t="inlineStr"/>
+      <c r="R5" s="6" t="inlineStr"/>
+      <c r="S5" s="6" t="inlineStr"/>
+      <c r="T5" s="6" t="inlineStr"/>
+      <c r="U5" s="6" t="inlineStr"/>
+      <c r="V5" s="6" t="inlineStr"/>
+      <c r="W5" s="6" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>900</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>21.02.2025</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>СДЭК</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>1 продуктов</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>0 осн.</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
+      <c r="I6" s="3" t="inlineStr"/>
+      <c r="J6" s="3" t="inlineStr"/>
+      <c r="K6" s="4" t="inlineStr">
         <is>
           <t>Закрыт</t>
         </is>
       </c>
-      <c r="L5" s="4" t="inlineStr">
+      <c r="L6" s="4" t="inlineStr">
         <is>
           <t>Леша разраб (@Ni3omi)</t>
         </is>
       </c>
-      <c r="M5" s="4" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="N5" s="3" t="inlineStr"/>
-      <c r="O5" s="3" t="inlineStr"/>
-      <c r="P5" s="3" t="n"/>
-      <c r="Q5" s="3" t="n"/>
-      <c r="R5" s="3" t="n">
-        <v>800</v>
-      </c>
-      <c r="S5" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="T5" s="3" t="n">
+      <c r="M6" s="3" t="inlineStr"/>
+      <c r="N6" s="3" t="inlineStr"/>
+      <c r="O6" s="3" t="inlineStr"/>
+      <c r="P6" s="3" t="n"/>
+      <c r="Q6" s="3" t="n"/>
+      <c r="R6" s="3" t="n">
+        <v>200</v>
+      </c>
+      <c r="S6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U5" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="V5" s="3" t="n">
+      <c r="T6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="W5" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" outlineLevel="1">
-      <c r="A6" s="5" t="n">
-        <v>898</v>
-      </c>
-      <c r="B6" s="6" t="inlineStr">
-        <is>
-          <t>09.12.2024</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>Прямая</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>Таежная</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>Да</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="inlineStr">
-        <is>
-          <t>Закрыт</t>
-        </is>
-      </c>
-      <c r="H6" s="6" t="n"/>
-      <c r="I6" s="6" t="inlineStr"/>
-      <c r="J6" s="6" t="inlineStr"/>
-      <c r="K6" s="7" t="inlineStr">
-        <is>
-          <t>Закрыт</t>
-        </is>
-      </c>
-      <c r="L6" s="7" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="M6" s="7" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="N6" s="6" t="inlineStr"/>
-      <c r="O6" s="6" t="inlineStr"/>
-      <c r="P6" s="6" t="inlineStr"/>
-      <c r="Q6" s="6" t="inlineStr"/>
-      <c r="R6" s="6" t="inlineStr"/>
-      <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" s="6" t="inlineStr"/>
-      <c r="U6" s="6" t="inlineStr"/>
-      <c r="V6" s="6" t="inlineStr"/>
-      <c r="W6" s="6" t="inlineStr"/>
+      <c r="U6" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="V6" s="3" t="n"/>
+      <c r="W6" s="3" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" s="5" t="n">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>09.12.2024</t>
+          <t>21.02.2025</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Прямая</t>
+          <t>СДЭК</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>Гирлянда роса</t>
+          <t>Корзинка белая</t>
         </is>
       </c>
       <c r="E7" s="6" t="inlineStr">
         <is>
-          <t>100м</t>
+          <t>2990 - 4 части</t>
         </is>
       </c>
       <c r="F7" s="6" t="inlineStr">
@@ -1028,11 +1022,7 @@
           <t>Леша разраб (@Ni3omi)</t>
         </is>
       </c>
-      <c r="M7" s="7" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
+      <c r="M7" s="6" t="inlineStr"/>
       <c r="N7" s="6" t="inlineStr"/>
       <c r="O7" s="6" t="inlineStr"/>
       <c r="P7" s="6" t="inlineStr"/>
@@ -1044,215 +1034,85 @@
       <c r="V7" s="6" t="inlineStr"/>
       <c r="W7" s="6" t="inlineStr"/>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>897</v>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>09.12.2024</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>Прямая</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>1 продуктов</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr"/>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>1 осн.</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr"/>
-      <c r="H8" s="3" t="inlineStr"/>
-      <c r="I8" s="3" t="inlineStr"/>
-      <c r="J8" s="3" t="inlineStr"/>
-      <c r="K8" s="4" t="inlineStr">
-        <is>
-          <t>Закрыт</t>
-        </is>
-      </c>
-      <c r="L8" s="4" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="M8" s="4" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="N8" s="3" t="inlineStr"/>
-      <c r="O8" s="3" t="inlineStr"/>
-      <c r="P8" s="3" t="n"/>
-      <c r="Q8" s="3" t="n"/>
-      <c r="R8" s="3" t="n">
-        <v>800</v>
-      </c>
-      <c r="S8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" s="3" t="n">
-        <v>300</v>
-      </c>
-      <c r="V8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" outlineLevel="1">
-      <c r="A9" s="5" t="n">
-        <v>897</v>
-      </c>
-      <c r="B9" s="6" t="inlineStr">
-        <is>
-          <t>09.12.2024</t>
-        </is>
-      </c>
-      <c r="C9" s="6" t="inlineStr">
-        <is>
-          <t>Прямая</t>
-        </is>
-      </c>
-      <c r="D9" s="6" t="inlineStr">
-        <is>
-          <t>Королевская</t>
-        </is>
-      </c>
-      <c r="E9" s="6" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="F9" s="6" t="inlineStr">
-        <is>
-          <t>Да</t>
-        </is>
-      </c>
-      <c r="G9" s="6" t="inlineStr">
-        <is>
-          <t>Закрыт</t>
-        </is>
-      </c>
-      <c r="H9" s="6" t="n"/>
-      <c r="I9" s="6" t="inlineStr"/>
-      <c r="J9" s="6" t="inlineStr"/>
-      <c r="K9" s="7" t="inlineStr">
-        <is>
-          <t>Закрыт</t>
-        </is>
-      </c>
-      <c r="L9" s="7" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="M9" s="7" t="inlineStr">
-        <is>
-          <t>Леша разраб (@Ni3omi)</t>
-        </is>
-      </c>
-      <c r="N9" s="6" t="inlineStr"/>
-      <c r="O9" s="6" t="inlineStr"/>
-      <c r="P9" s="6" t="inlineStr"/>
-      <c r="Q9" s="6" t="inlineStr"/>
-      <c r="R9" s="6" t="inlineStr"/>
-      <c r="S9" s="6" t="inlineStr"/>
-      <c r="T9" s="6" t="inlineStr"/>
-      <c r="U9" s="6" t="inlineStr"/>
-      <c r="V9" s="6" t="inlineStr"/>
-      <c r="W9" s="6" t="inlineStr"/>
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>ИТОГИ:</t>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
+        <is>
+          <t>Всего основных продуктов:</t>
+        </is>
+      </c>
+      <c r="D10" s="10">
+        <f>SUMPRODUCT(SUBTOTAL(3,OFFSET(F2,ROW(F2:F8)-ROW(F2),0)),--(F2:F8="Да"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="9" t="inlineStr">
+        <is>
+          <t>Сумма оплаты менеджерам:</t>
+        </is>
+      </c>
+      <c r="D11" s="10">
+        <f>SUBTOTAL(9,R2:R8)</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="inlineStr">
-        <is>
-          <t>ИТОГИ:</t>
-        </is>
-      </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>Всего основных продуктов:</t>
+          <t>Сумма оплаты показавшим:</t>
         </is>
       </c>
       <c r="D12" s="10">
-        <f>SUMPRODUCT(SUBTOTAL(3,OFFSET(F2,ROW(F2:F10)-ROW(F2),0)),--(F2:F10="Да"))</f>
+        <f>SUBTOTAL(9,S2:S8)</f>
         <v/>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="9" t="inlineStr">
         <is>
-          <t>Сумма оплаты менеджерам:</t>
+          <t>Сумма оплаты упаковщикам:</t>
         </is>
       </c>
       <c r="D13" s="10">
-        <f>SUBTOTAL(9,R2:R10)</f>
+        <f>SUBTOTAL(9,T2:T8)</f>
         <v/>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="9" t="inlineStr">
         <is>
-          <t>Сумма оплаты показавшим:</t>
+          <t>Сумма продаж итоговая:</t>
         </is>
       </c>
       <c r="D14" s="10">
-        <f>SUBTOTAL(9,S2:S10)</f>
+        <f>SUBTOTAL(9,U2:U8)</f>
         <v/>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="9" t="inlineStr">
         <is>
-          <t>Сумма оплаты упаковщикам:</t>
+          <t>Сумма доставки итоговая:</t>
         </is>
       </c>
       <c r="D15" s="10">
-        <f>SUBTOTAL(9,T2:T10)</f>
+        <f>SUBTOTAL(9,V2:V8)</f>
         <v/>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="9" t="inlineStr">
         <is>
-          <t>Сумма продаж итоговая:</t>
+          <t>Итоговая сумма:</t>
         </is>
       </c>
       <c r="D16" s="10">
-        <f>SUBTOTAL(9,U2:U10)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" s="9" t="inlineStr">
-        <is>
-          <t>Сумма доставки итоговая:</t>
-        </is>
-      </c>
-      <c r="D17" s="10">
-        <f>SUBTOTAL(9,V2:V10)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="9" t="inlineStr">
-        <is>
-          <t>Итоговая сумма:</t>
-        </is>
-      </c>
-      <c r="D18" s="10">
-        <f>SUBTOTAL(9,W2:W10)</f>
+        <f>SUBTOTAL(9,W2:W8)</f>
         <v/>
       </c>
     </row>

</xml_diff>